<commit_message>
Updated 07 Dec with cumulative stats
</commit_message>
<xml_diff>
--- a/Game-data/WBBGame stats.xlsx
+++ b/Game-data/WBBGame stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loganclarke/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F316AA-2DDA-3B45-AAE3-5A72EC5A0B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50DAB4A-9829-9349-BA63-0CA743867804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{183A49D1-7E17-DF4D-9FDB-8B4A46151E55}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="8" xr2:uid="{183A49D1-7E17-DF4D-9FDB-8B4A46151E55}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1 Games" sheetId="3" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Week 3 Total" sheetId="8" r:id="rId6"/>
     <sheet name="Week 4 Games" sheetId="9" r:id="rId7"/>
     <sheet name="Week 4 Total" sheetId="10" r:id="rId8"/>
+    <sheet name="Cumulative Total" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="68">
   <si>
     <t>MP</t>
   </si>
@@ -16812,7 +16813,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
@@ -18899,4 +18900,2338 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F10DA945-26CA-3B44-A417-635691B7D62C}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:AJ17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AJ25" sqref="AJ25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="4">
+        <f>SUM('Week 1 Total'!C2,'Week 2 Total'!C2,'Week 3 Total'!C2,'Week 4 Total'!C2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <f>SUM('Week 1 Total'!D2,'Week 2 Total'!D2,'Week 3 Total'!D2,'Week 4 Total'!D2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <f>SUM('Week 1 Total'!E2,'Week 2 Total'!E2,'Week 3 Total'!E2,'Week 4 Total'!E2)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <f>SUM('Week 1 Total'!F2,'Week 2 Total'!F2,'Week 3 Total'!F2,'Week 4 Total'!F2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <f>SUM('Week 1 Total'!G2,'Week 2 Total'!G2,'Week 3 Total'!G2,'Week 4 Total'!G2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <f>SUM('Week 1 Total'!H2,'Week 2 Total'!H2,'Week 3 Total'!H2,'Week 4 Total'!H2)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <f>SUM('Week 1 Total'!I2,'Week 2 Total'!I2,'Week 3 Total'!I2,'Week 4 Total'!I2)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="4" t="str">
+        <f>IF(ISERROR(H2/I2),"N/A",H2/I2)</f>
+        <v>N/A</v>
+      </c>
+      <c r="K2" s="4">
+        <f>SUM('Week 1 Total'!K2,'Week 2 Total'!K2,'Week 3 Total'!K2,'Week 4 Total'!K2)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <f>SUM('Week 1 Total'!L2,'Week 2 Total'!L2,'Week 3 Total'!L2,'Week 4 Total'!L2)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <f>SUM('Week 1 Total'!M2,'Week 2 Total'!M2,'Week 3 Total'!M2,'Week 4 Total'!M2)</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <f>SUM('Week 1 Total'!N2,'Week 2 Total'!N2,'Week 3 Total'!N2,'Week 4 Total'!N2)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <f>SUM('Week 1 Total'!O2,'Week 2 Total'!O2,'Week 3 Total'!O2,'Week 4 Total'!O2)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="4">
+        <f>SUM('Week 1 Total'!P2,'Week 2 Total'!P2,'Week 3 Total'!P2,'Week 4 Total'!P2)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4">
+        <f>SUM('Week 1 Total'!Q2,'Week 2 Total'!Q2,'Week 3 Total'!Q2,'Week 4 Total'!Q2)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="4">
+        <f>SUM('Week 1 Total'!R2,'Week 2 Total'!R2,'Week 3 Total'!R2,'Week 4 Total'!R2)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="4">
+        <f>SUM('Week 1 Total'!S2,'Week 2 Total'!S2,'Week 3 Total'!S2,'Week 4 Total'!S2)</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="4">
+        <f>SUM('Week 1 Total'!T2,'Week 2 Total'!T2,'Week 3 Total'!T2,'Week 4 Total'!T2)</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="2">
+        <f>IF(ISERROR(S2/R2),0,S2/R2)</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4">
+        <f>SUM('Week 1 Total'!W2,'Week 2 Total'!W2,'Week 3 Total'!W2,'Week 4 Total'!W2)</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="4">
+        <f>SUM('Week 1 Total'!X2,'Week 2 Total'!X2,'Week 3 Total'!X2,'Week 4 Total'!X2)</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="4">
+        <f>SUM('Week 1 Total'!Y2,'Week 2 Total'!Y2,'Week 3 Total'!Y2,'Week 4 Total'!Y2)</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2">
+        <f>IF(ISERROR(X2/W2),0,X2/W2)</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="4">
+        <f>SUM('Week 1 Total'!AA2,'Week 2 Total'!AA2,'Week 3 Total'!AA2,'Week 4 Total'!AA2)</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="4">
+        <f>SUM('Week 1 Total'!AB2,'Week 2 Total'!AB2,'Week 3 Total'!AB2,'Week 4 Total'!AB2)</f>
+        <v>0</v>
+      </c>
+      <c r="AC2" s="4">
+        <f>SUM('Week 1 Total'!AC2,'Week 2 Total'!AC2,'Week 3 Total'!AC2,'Week 4 Total'!AC2)</f>
+        <v>0</v>
+      </c>
+      <c r="AD2" s="2">
+        <f t="shared" ref="AD2:AD11" si="0">IF(ISERROR(AB2/AA2),0,AB2/AA2)</f>
+        <v>0</v>
+      </c>
+      <c r="AE2" s="4">
+        <f>SUM('Week 1 Total'!AE2,'Week 2 Total'!AE2,'Week 3 Total'!AE2,'Week 4 Total'!AE2)</f>
+        <v>0</v>
+      </c>
+      <c r="AF2" s="4">
+        <f>SUM('Week 1 Total'!AF2,'Week 2 Total'!AF2,'Week 3 Total'!AF2,'Week 4 Total'!AF2)</f>
+        <v>0</v>
+      </c>
+      <c r="AG2" s="4">
+        <f>SUM('Week 1 Total'!AG2,'Week 2 Total'!AG2,'Week 3 Total'!AG2,'Week 4 Total'!AG2)</f>
+        <v>0</v>
+      </c>
+      <c r="AH2" s="2">
+        <f>IF(ISERROR(AF2/AE2),0,AF2/AE2)</f>
+        <v>0</v>
+      </c>
+      <c r="AI2" s="4">
+        <f>SUM('Week 1 Total'!AI2,'Week 2 Total'!AI2,'Week 3 Total'!AI2,'Week 4 Total'!AI2)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="4">
+        <f>SUM('Week 1 Total'!AJ2,'Week 2 Total'!AJ2,'Week 3 Total'!AJ2,'Week 4 Total'!AJ2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4">
+        <f>SUM('Week 1 Total'!C3,'Week 2 Total'!C3,'Week 3 Total'!C3,'Week 4 Total'!C3)</f>
+        <v>250</v>
+      </c>
+      <c r="D3" s="4">
+        <f>SUM('Week 1 Total'!D3,'Week 2 Total'!D3,'Week 3 Total'!D3,'Week 4 Total'!D3)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <f>SUM('Week 1 Total'!E3,'Week 2 Total'!E3,'Week 3 Total'!E3,'Week 4 Total'!E3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <f>SUM('Week 1 Total'!F3,'Week 2 Total'!F3,'Week 3 Total'!F3,'Week 4 Total'!F3)</f>
+        <v>154</v>
+      </c>
+      <c r="G3" s="4">
+        <f>SUM('Week 1 Total'!G3,'Week 2 Total'!G3,'Week 3 Total'!G3,'Week 4 Total'!G3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <f>SUM('Week 1 Total'!H3,'Week 2 Total'!H3,'Week 3 Total'!H3,'Week 4 Total'!H3)</f>
+        <v>26</v>
+      </c>
+      <c r="I3" s="4">
+        <f>SUM('Week 1 Total'!I3,'Week 2 Total'!I3,'Week 3 Total'!I3,'Week 4 Total'!I3)</f>
+        <v>18</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J17" si="1">IF(ISERROR(H3/I3),"N/A",H3/I3)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K3" s="4">
+        <f>SUM('Week 1 Total'!K3,'Week 2 Total'!K3,'Week 3 Total'!K3,'Week 4 Total'!K3)</f>
+        <v>17</v>
+      </c>
+      <c r="L3" s="4">
+        <f>SUM('Week 1 Total'!L3,'Week 2 Total'!L3,'Week 3 Total'!L3,'Week 4 Total'!L3)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <f>SUM('Week 1 Total'!M3,'Week 2 Total'!M3,'Week 3 Total'!M3,'Week 4 Total'!M3)</f>
+        <v>3</v>
+      </c>
+      <c r="N3" s="4">
+        <f>SUM('Week 1 Total'!N3,'Week 2 Total'!N3,'Week 3 Total'!N3,'Week 4 Total'!N3)</f>
+        <v>40</v>
+      </c>
+      <c r="O3" s="4">
+        <f>SUM('Week 1 Total'!O3,'Week 2 Total'!O3,'Week 3 Total'!O3,'Week 4 Total'!O3)</f>
+        <v>13</v>
+      </c>
+      <c r="P3" s="4">
+        <f>SUM('Week 1 Total'!P3,'Week 2 Total'!P3,'Week 3 Total'!P3,'Week 4 Total'!P3)</f>
+        <v>27</v>
+      </c>
+      <c r="Q3" s="4">
+        <f>SUM('Week 1 Total'!Q3,'Week 2 Total'!Q3,'Week 3 Total'!Q3,'Week 4 Total'!Q3)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="4">
+        <f>SUM('Week 1 Total'!R3,'Week 2 Total'!R3,'Week 3 Total'!R3,'Week 4 Total'!R3)</f>
+        <v>111</v>
+      </c>
+      <c r="S3" s="4">
+        <f>SUM('Week 1 Total'!S3,'Week 2 Total'!S3,'Week 3 Total'!S3,'Week 4 Total'!S3)</f>
+        <v>55</v>
+      </c>
+      <c r="T3" s="4">
+        <f>SUM('Week 1 Total'!T3,'Week 2 Total'!T3,'Week 3 Total'!T3,'Week 4 Total'!T3)</f>
+        <v>56</v>
+      </c>
+      <c r="U3" s="2">
+        <f t="shared" ref="U3:U17" si="2">IF(ISERROR(S3/R3),0,S3/R3)</f>
+        <v>0.49549549549549549</v>
+      </c>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4">
+        <f>SUM('Week 1 Total'!W3,'Week 2 Total'!W3,'Week 3 Total'!W3,'Week 4 Total'!W3)</f>
+        <v>79</v>
+      </c>
+      <c r="X3" s="4">
+        <f>SUM('Week 1 Total'!X3,'Week 2 Total'!X3,'Week 3 Total'!X3,'Week 4 Total'!X3)</f>
+        <v>48</v>
+      </c>
+      <c r="Y3" s="4">
+        <f>SUM('Week 1 Total'!Y3,'Week 2 Total'!Y3,'Week 3 Total'!Y3,'Week 4 Total'!Y3)</f>
+        <v>31</v>
+      </c>
+      <c r="Z3" s="2">
+        <f t="shared" ref="Z3:Z17" si="3">IF(ISERROR(X3/W3),0,X3/W3)</f>
+        <v>0.60759493670886078</v>
+      </c>
+      <c r="AA3" s="4">
+        <f>SUM('Week 1 Total'!AA3,'Week 2 Total'!AA3,'Week 3 Total'!AA3,'Week 4 Total'!AA3)</f>
+        <v>32</v>
+      </c>
+      <c r="AB3" s="4">
+        <f>SUM('Week 1 Total'!AB3,'Week 2 Total'!AB3,'Week 3 Total'!AB3,'Week 4 Total'!AB3)</f>
+        <v>7</v>
+      </c>
+      <c r="AC3" s="4">
+        <f>SUM('Week 1 Total'!AC3,'Week 2 Total'!AC3,'Week 3 Total'!AC3,'Week 4 Total'!AC3)</f>
+        <v>25</v>
+      </c>
+      <c r="AD3" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21875</v>
+      </c>
+      <c r="AE3" s="4">
+        <f>SUM('Week 1 Total'!AE3,'Week 2 Total'!AE3,'Week 3 Total'!AE3,'Week 4 Total'!AE3)</f>
+        <v>43</v>
+      </c>
+      <c r="AF3" s="4">
+        <f>SUM('Week 1 Total'!AF3,'Week 2 Total'!AF3,'Week 3 Total'!AF3,'Week 4 Total'!AF3)</f>
+        <v>37</v>
+      </c>
+      <c r="AG3" s="4">
+        <f>SUM('Week 1 Total'!AG3,'Week 2 Total'!AG3,'Week 3 Total'!AG3,'Week 4 Total'!AG3)</f>
+        <v>6</v>
+      </c>
+      <c r="AH3" s="2">
+        <f t="shared" ref="AH3:AH17" si="4">IF(ISERROR(AF3/AE3),0,AF3/AE3)</f>
+        <v>0.86046511627906974</v>
+      </c>
+      <c r="AI3" s="4">
+        <f>SUM('Week 1 Total'!AI3,'Week 2 Total'!AI3,'Week 3 Total'!AI3,'Week 4 Total'!AI3)</f>
+        <v>3</v>
+      </c>
+      <c r="AJ3" s="4">
+        <f>SUM('Week 1 Total'!AJ3,'Week 2 Total'!AJ3,'Week 3 Total'!AJ3,'Week 4 Total'!AJ3)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4">
+        <f>SUM('Week 1 Total'!C4,'Week 2 Total'!C4,'Week 3 Total'!C4,'Week 4 Total'!C4)</f>
+        <v>100</v>
+      </c>
+      <c r="D4" s="4">
+        <f>SUM('Week 1 Total'!D4,'Week 2 Total'!D4,'Week 3 Total'!D4,'Week 4 Total'!D4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <f>SUM('Week 1 Total'!E4,'Week 2 Total'!E4,'Week 3 Total'!E4,'Week 4 Total'!E4)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <f>SUM('Week 1 Total'!F4,'Week 2 Total'!F4,'Week 3 Total'!F4,'Week 4 Total'!F4)</f>
+        <v>25</v>
+      </c>
+      <c r="G4" s="4">
+        <f>SUM('Week 1 Total'!G4,'Week 2 Total'!G4,'Week 3 Total'!G4,'Week 4 Total'!G4)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <f>SUM('Week 1 Total'!H4,'Week 2 Total'!H4,'Week 3 Total'!H4,'Week 4 Total'!H4)</f>
+        <v>5</v>
+      </c>
+      <c r="I4" s="4">
+        <f>SUM('Week 1 Total'!I4,'Week 2 Total'!I4,'Week 3 Total'!I4,'Week 4 Total'!I4)</f>
+        <v>8</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+      <c r="K4" s="4">
+        <f>SUM('Week 1 Total'!K4,'Week 2 Total'!K4,'Week 3 Total'!K4,'Week 4 Total'!K4)</f>
+        <v>6</v>
+      </c>
+      <c r="L4" s="4">
+        <f>SUM('Week 1 Total'!L4,'Week 2 Total'!L4,'Week 3 Total'!L4,'Week 4 Total'!L4)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <f>SUM('Week 1 Total'!M4,'Week 2 Total'!M4,'Week 3 Total'!M4,'Week 4 Total'!M4)</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="4">
+        <f>SUM('Week 1 Total'!N4,'Week 2 Total'!N4,'Week 3 Total'!N4,'Week 4 Total'!N4)</f>
+        <v>16</v>
+      </c>
+      <c r="O4" s="4">
+        <f>SUM('Week 1 Total'!O4,'Week 2 Total'!O4,'Week 3 Total'!O4,'Week 4 Total'!O4)</f>
+        <v>1</v>
+      </c>
+      <c r="P4" s="4">
+        <f>SUM('Week 1 Total'!P4,'Week 2 Total'!P4,'Week 3 Total'!P4,'Week 4 Total'!P4)</f>
+        <v>15</v>
+      </c>
+      <c r="Q4" s="4">
+        <f>SUM('Week 1 Total'!Q4,'Week 2 Total'!Q4,'Week 3 Total'!Q4,'Week 4 Total'!Q4)</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <f>SUM('Week 1 Total'!R4,'Week 2 Total'!R4,'Week 3 Total'!R4,'Week 4 Total'!R4)</f>
+        <v>19</v>
+      </c>
+      <c r="S4" s="4">
+        <f>SUM('Week 1 Total'!S4,'Week 2 Total'!S4,'Week 3 Total'!S4,'Week 4 Total'!S4)</f>
+        <v>8</v>
+      </c>
+      <c r="T4" s="4">
+        <f>SUM('Week 1 Total'!T4,'Week 2 Total'!T4,'Week 3 Total'!T4,'Week 4 Total'!T4)</f>
+        <v>11</v>
+      </c>
+      <c r="U4" s="2">
+        <f t="shared" si="2"/>
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4">
+        <f>SUM('Week 1 Total'!W4,'Week 2 Total'!W4,'Week 3 Total'!W4,'Week 4 Total'!W4)</f>
+        <v>7</v>
+      </c>
+      <c r="X4" s="4">
+        <f>SUM('Week 1 Total'!X4,'Week 2 Total'!X4,'Week 3 Total'!X4,'Week 4 Total'!X4)</f>
+        <v>1</v>
+      </c>
+      <c r="Y4" s="4">
+        <f>SUM('Week 1 Total'!Y4,'Week 2 Total'!Y4,'Week 3 Total'!Y4,'Week 4 Total'!Y4)</f>
+        <v>6</v>
+      </c>
+      <c r="Z4" s="2">
+        <f t="shared" si="3"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA4" s="4">
+        <f>SUM('Week 1 Total'!AA4,'Week 2 Total'!AA4,'Week 3 Total'!AA4,'Week 4 Total'!AA4)</f>
+        <v>12</v>
+      </c>
+      <c r="AB4" s="4">
+        <f>SUM('Week 1 Total'!AB4,'Week 2 Total'!AB4,'Week 3 Total'!AB4,'Week 4 Total'!AB4)</f>
+        <v>7</v>
+      </c>
+      <c r="AC4" s="4">
+        <f>SUM('Week 1 Total'!AC4,'Week 2 Total'!AC4,'Week 3 Total'!AC4,'Week 4 Total'!AC4)</f>
+        <v>5</v>
+      </c>
+      <c r="AD4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="AE4" s="4">
+        <f>SUM('Week 1 Total'!AE4,'Week 2 Total'!AE4,'Week 3 Total'!AE4,'Week 4 Total'!AE4)</f>
+        <v>2</v>
+      </c>
+      <c r="AF4" s="4">
+        <f>SUM('Week 1 Total'!AF4,'Week 2 Total'!AF4,'Week 3 Total'!AF4,'Week 4 Total'!AF4)</f>
+        <v>2</v>
+      </c>
+      <c r="AG4" s="4">
+        <f>SUM('Week 1 Total'!AG4,'Week 2 Total'!AG4,'Week 3 Total'!AG4,'Week 4 Total'!AG4)</f>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AI4" s="4">
+        <f>SUM('Week 1 Total'!AI4,'Week 2 Total'!AI4,'Week 3 Total'!AI4,'Week 4 Total'!AI4)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="4">
+        <f>SUM('Week 1 Total'!AJ4,'Week 2 Total'!AJ4,'Week 3 Total'!AJ4,'Week 4 Total'!AJ4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4">
+        <f>SUM('Week 1 Total'!C5,'Week 2 Total'!C5,'Week 3 Total'!C5,'Week 4 Total'!C5)</f>
+        <v>40</v>
+      </c>
+      <c r="D5" s="4">
+        <f>SUM('Week 1 Total'!D5,'Week 2 Total'!D5,'Week 3 Total'!D5,'Week 4 Total'!D5)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <f>SUM('Week 1 Total'!E5,'Week 2 Total'!E5,'Week 3 Total'!E5,'Week 4 Total'!E5)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <f>SUM('Week 1 Total'!F5,'Week 2 Total'!F5,'Week 3 Total'!F5,'Week 4 Total'!F5)</f>
+        <v>6</v>
+      </c>
+      <c r="G5" s="4">
+        <f>SUM('Week 1 Total'!G5,'Week 2 Total'!G5,'Week 3 Total'!G5,'Week 4 Total'!G5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <f>SUM('Week 1 Total'!H5,'Week 2 Total'!H5,'Week 3 Total'!H5,'Week 4 Total'!H5)</f>
+        <v>6</v>
+      </c>
+      <c r="I5" s="4">
+        <f>SUM('Week 1 Total'!I5,'Week 2 Total'!I5,'Week 3 Total'!I5,'Week 4 Total'!I5)</f>
+        <v>6</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <f>SUM('Week 1 Total'!K5,'Week 2 Total'!K5,'Week 3 Total'!K5,'Week 4 Total'!K5)</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
+        <f>SUM('Week 1 Total'!L5,'Week 2 Total'!L5,'Week 3 Total'!L5,'Week 4 Total'!L5)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <f>SUM('Week 1 Total'!M5,'Week 2 Total'!M5,'Week 3 Total'!M5,'Week 4 Total'!M5)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <f>SUM('Week 1 Total'!N5,'Week 2 Total'!N5,'Week 3 Total'!N5,'Week 4 Total'!N5)</f>
+        <v>4</v>
+      </c>
+      <c r="O5" s="4">
+        <f>SUM('Week 1 Total'!O5,'Week 2 Total'!O5,'Week 3 Total'!O5,'Week 4 Total'!O5)</f>
+        <v>2</v>
+      </c>
+      <c r="P5" s="4">
+        <f>SUM('Week 1 Total'!P5,'Week 2 Total'!P5,'Week 3 Total'!P5,'Week 4 Total'!P5)</f>
+        <v>2</v>
+      </c>
+      <c r="Q5" s="4">
+        <f>SUM('Week 1 Total'!Q5,'Week 2 Total'!Q5,'Week 3 Total'!Q5,'Week 4 Total'!Q5)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="4">
+        <f>SUM('Week 1 Total'!R5,'Week 2 Total'!R5,'Week 3 Total'!R5,'Week 4 Total'!R5)</f>
+        <v>11</v>
+      </c>
+      <c r="S5" s="4">
+        <f>SUM('Week 1 Total'!S5,'Week 2 Total'!S5,'Week 3 Total'!S5,'Week 4 Total'!S5)</f>
+        <v>2</v>
+      </c>
+      <c r="T5" s="4">
+        <f>SUM('Week 1 Total'!T5,'Week 2 Total'!T5,'Week 3 Total'!T5,'Week 4 Total'!T5)</f>
+        <v>9</v>
+      </c>
+      <c r="U5" s="2">
+        <f t="shared" si="2"/>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4">
+        <f>SUM('Week 1 Total'!W5,'Week 2 Total'!W5,'Week 3 Total'!W5,'Week 4 Total'!W5)</f>
+        <v>6</v>
+      </c>
+      <c r="X5" s="4">
+        <f>SUM('Week 1 Total'!X5,'Week 2 Total'!X5,'Week 3 Total'!X5,'Week 4 Total'!X5)</f>
+        <v>2</v>
+      </c>
+      <c r="Y5" s="4">
+        <f>SUM('Week 1 Total'!Y5,'Week 2 Total'!Y5,'Week 3 Total'!Y5,'Week 4 Total'!Y5)</f>
+        <v>4</v>
+      </c>
+      <c r="Z5" s="2">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA5" s="4">
+        <f>SUM('Week 1 Total'!AA5,'Week 2 Total'!AA5,'Week 3 Total'!AA5,'Week 4 Total'!AA5)</f>
+        <v>5</v>
+      </c>
+      <c r="AB5" s="4">
+        <f>SUM('Week 1 Total'!AB5,'Week 2 Total'!AB5,'Week 3 Total'!AB5,'Week 4 Total'!AB5)</f>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="4">
+        <f>SUM('Week 1 Total'!AC5,'Week 2 Total'!AC5,'Week 3 Total'!AC5,'Week 4 Total'!AC5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE5" s="4">
+        <f>SUM('Week 1 Total'!AE5,'Week 2 Total'!AE5,'Week 3 Total'!AE5,'Week 4 Total'!AE5)</f>
+        <v>2</v>
+      </c>
+      <c r="AF5" s="4">
+        <f>SUM('Week 1 Total'!AF5,'Week 2 Total'!AF5,'Week 3 Total'!AF5,'Week 4 Total'!AF5)</f>
+        <v>2</v>
+      </c>
+      <c r="AG5" s="4">
+        <f>SUM('Week 1 Total'!AG5,'Week 2 Total'!AG5,'Week 3 Total'!AG5,'Week 4 Total'!AG5)</f>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AI5" s="4">
+        <f>SUM('Week 1 Total'!AI5,'Week 2 Total'!AI5,'Week 3 Total'!AI5,'Week 4 Total'!AI5)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="4">
+        <f>SUM('Week 1 Total'!AJ5,'Week 2 Total'!AJ5,'Week 3 Total'!AJ5,'Week 4 Total'!AJ5)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4">
+        <f>SUM('Week 1 Total'!C6,'Week 2 Total'!C6,'Week 3 Total'!C6,'Week 4 Total'!C6)</f>
+        <v>222</v>
+      </c>
+      <c r="D6" s="4">
+        <f>SUM('Week 1 Total'!D6,'Week 2 Total'!D6,'Week 3 Total'!D6,'Week 4 Total'!D6)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <f>SUM('Week 1 Total'!E6,'Week 2 Total'!E6,'Week 3 Total'!E6,'Week 4 Total'!E6)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <f>SUM('Week 1 Total'!F6,'Week 2 Total'!F6,'Week 3 Total'!F6,'Week 4 Total'!F6)</f>
+        <v>33</v>
+      </c>
+      <c r="G6" s="4">
+        <f>SUM('Week 1 Total'!G6,'Week 2 Total'!G6,'Week 3 Total'!G6,'Week 4 Total'!G6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <f>SUM('Week 1 Total'!H6,'Week 2 Total'!H6,'Week 3 Total'!H6,'Week 4 Total'!H6)</f>
+        <v>33</v>
+      </c>
+      <c r="I6" s="4">
+        <f>SUM('Week 1 Total'!I6,'Week 2 Total'!I6,'Week 3 Total'!I6,'Week 4 Total'!I6)</f>
+        <v>14</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="1"/>
+        <v>2.3571428571428572</v>
+      </c>
+      <c r="K6" s="4">
+        <f>SUM('Week 1 Total'!K6,'Week 2 Total'!K6,'Week 3 Total'!K6,'Week 4 Total'!K6)</f>
+        <v>7</v>
+      </c>
+      <c r="L6" s="4">
+        <f>SUM('Week 1 Total'!L6,'Week 2 Total'!L6,'Week 3 Total'!L6,'Week 4 Total'!L6)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <f>SUM('Week 1 Total'!M6,'Week 2 Total'!M6,'Week 3 Total'!M6,'Week 4 Total'!M6)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <f>SUM('Week 1 Total'!N6,'Week 2 Total'!N6,'Week 3 Total'!N6,'Week 4 Total'!N6)</f>
+        <v>22</v>
+      </c>
+      <c r="O6" s="4">
+        <f>SUM('Week 1 Total'!O6,'Week 2 Total'!O6,'Week 3 Total'!O6,'Week 4 Total'!O6)</f>
+        <v>1</v>
+      </c>
+      <c r="P6" s="4">
+        <f>SUM('Week 1 Total'!P6,'Week 2 Total'!P6,'Week 3 Total'!P6,'Week 4 Total'!P6)</f>
+        <v>21</v>
+      </c>
+      <c r="Q6" s="4">
+        <f>SUM('Week 1 Total'!Q6,'Week 2 Total'!Q6,'Week 3 Total'!Q6,'Week 4 Total'!Q6)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="4">
+        <f>SUM('Week 1 Total'!R6,'Week 2 Total'!R6,'Week 3 Total'!R6,'Week 4 Total'!R6)</f>
+        <v>34</v>
+      </c>
+      <c r="S6" s="4">
+        <f>SUM('Week 1 Total'!S6,'Week 2 Total'!S6,'Week 3 Total'!S6,'Week 4 Total'!S6)</f>
+        <v>13</v>
+      </c>
+      <c r="T6" s="4">
+        <f>SUM('Week 1 Total'!T6,'Week 2 Total'!T6,'Week 3 Total'!T6,'Week 4 Total'!T6)</f>
+        <v>21</v>
+      </c>
+      <c r="U6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.38235294117647056</v>
+      </c>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4">
+        <f>SUM('Week 1 Total'!W6,'Week 2 Total'!W6,'Week 3 Total'!W6,'Week 4 Total'!W6)</f>
+        <v>25</v>
+      </c>
+      <c r="X6" s="4">
+        <f>SUM('Week 1 Total'!X6,'Week 2 Total'!X6,'Week 3 Total'!X6,'Week 4 Total'!X6)</f>
+        <v>9</v>
+      </c>
+      <c r="Y6" s="4">
+        <f>SUM('Week 1 Total'!Y6,'Week 2 Total'!Y6,'Week 3 Total'!Y6,'Week 4 Total'!Y6)</f>
+        <v>16</v>
+      </c>
+      <c r="Z6" s="2">
+        <f t="shared" si="3"/>
+        <v>0.36</v>
+      </c>
+      <c r="AA6" s="4">
+        <f>SUM('Week 1 Total'!AA6,'Week 2 Total'!AA6,'Week 3 Total'!AA6,'Week 4 Total'!AA6)</f>
+        <v>9</v>
+      </c>
+      <c r="AB6" s="4">
+        <f>SUM('Week 1 Total'!AB6,'Week 2 Total'!AB6,'Week 3 Total'!AB6,'Week 4 Total'!AB6)</f>
+        <v>4</v>
+      </c>
+      <c r="AC6" s="4">
+        <f>SUM('Week 1 Total'!AC6,'Week 2 Total'!AC6,'Week 3 Total'!AC6,'Week 4 Total'!AC6)</f>
+        <v>5</v>
+      </c>
+      <c r="AD6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="AE6" s="4">
+        <f>SUM('Week 1 Total'!AE6,'Week 2 Total'!AE6,'Week 3 Total'!AE6,'Week 4 Total'!AE6)</f>
+        <v>4</v>
+      </c>
+      <c r="AF6" s="4">
+        <f>SUM('Week 1 Total'!AF6,'Week 2 Total'!AF6,'Week 3 Total'!AF6,'Week 4 Total'!AF6)</f>
+        <v>3</v>
+      </c>
+      <c r="AG6" s="4">
+        <f>SUM('Week 1 Total'!AG6,'Week 2 Total'!AG6,'Week 3 Total'!AG6,'Week 4 Total'!AG6)</f>
+        <v>1</v>
+      </c>
+      <c r="AH6" s="2">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="AI6" s="4">
+        <f>SUM('Week 1 Total'!AI6,'Week 2 Total'!AI6,'Week 3 Total'!AI6,'Week 4 Total'!AI6)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="4">
+        <f>SUM('Week 1 Total'!AJ6,'Week 2 Total'!AJ6,'Week 3 Total'!AJ6,'Week 4 Total'!AJ6)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4">
+        <f>SUM('Week 1 Total'!C7,'Week 2 Total'!C7,'Week 3 Total'!C7,'Week 4 Total'!C7)</f>
+        <v>250</v>
+      </c>
+      <c r="D7" s="4">
+        <f>SUM('Week 1 Total'!D7,'Week 2 Total'!D7,'Week 3 Total'!D7,'Week 4 Total'!D7)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <f>SUM('Week 1 Total'!E7,'Week 2 Total'!E7,'Week 3 Total'!E7,'Week 4 Total'!E7)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <f>SUM('Week 1 Total'!F7,'Week 2 Total'!F7,'Week 3 Total'!F7,'Week 4 Total'!F7)</f>
+        <v>76</v>
+      </c>
+      <c r="G7" s="4">
+        <f>SUM('Week 1 Total'!G7,'Week 2 Total'!G7,'Week 3 Total'!G7,'Week 4 Total'!G7)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <f>SUM('Week 1 Total'!H7,'Week 2 Total'!H7,'Week 3 Total'!H7,'Week 4 Total'!H7)</f>
+        <v>41</v>
+      </c>
+      <c r="I7" s="4">
+        <f>SUM('Week 1 Total'!I7,'Week 2 Total'!I7,'Week 3 Total'!I7,'Week 4 Total'!I7)</f>
+        <v>20</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="K7" s="4">
+        <f>SUM('Week 1 Total'!K7,'Week 2 Total'!K7,'Week 3 Total'!K7,'Week 4 Total'!K7)</f>
+        <v>17</v>
+      </c>
+      <c r="L7" s="4">
+        <f>SUM('Week 1 Total'!L7,'Week 2 Total'!L7,'Week 3 Total'!L7,'Week 4 Total'!L7)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <f>SUM('Week 1 Total'!M7,'Week 2 Total'!M7,'Week 3 Total'!M7,'Week 4 Total'!M7)</f>
+        <v>9</v>
+      </c>
+      <c r="N7" s="4">
+        <f>SUM('Week 1 Total'!N7,'Week 2 Total'!N7,'Week 3 Total'!N7,'Week 4 Total'!N7)</f>
+        <v>23</v>
+      </c>
+      <c r="O7" s="4">
+        <f>SUM('Week 1 Total'!O7,'Week 2 Total'!O7,'Week 3 Total'!O7,'Week 4 Total'!O7)</f>
+        <v>5</v>
+      </c>
+      <c r="P7" s="4">
+        <f>SUM('Week 1 Total'!P7,'Week 2 Total'!P7,'Week 3 Total'!P7,'Week 4 Total'!P7)</f>
+        <v>18</v>
+      </c>
+      <c r="Q7" s="4">
+        <f>SUM('Week 1 Total'!Q7,'Week 2 Total'!Q7,'Week 3 Total'!Q7,'Week 4 Total'!Q7)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
+        <f>SUM('Week 1 Total'!R7,'Week 2 Total'!R7,'Week 3 Total'!R7,'Week 4 Total'!R7)</f>
+        <v>61</v>
+      </c>
+      <c r="S7" s="4">
+        <f>SUM('Week 1 Total'!S7,'Week 2 Total'!S7,'Week 3 Total'!S7,'Week 4 Total'!S7)</f>
+        <v>26</v>
+      </c>
+      <c r="T7" s="4">
+        <f>SUM('Week 1 Total'!T7,'Week 2 Total'!T7,'Week 3 Total'!T7,'Week 4 Total'!T7)</f>
+        <v>35</v>
+      </c>
+      <c r="U7" s="2">
+        <f t="shared" si="2"/>
+        <v>0.42622950819672129</v>
+      </c>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4">
+        <f>SUM('Week 1 Total'!W7,'Week 2 Total'!W7,'Week 3 Total'!W7,'Week 4 Total'!W7)</f>
+        <v>16</v>
+      </c>
+      <c r="X7" s="4">
+        <f>SUM('Week 1 Total'!X7,'Week 2 Total'!X7,'Week 3 Total'!X7,'Week 4 Total'!X7)</f>
+        <v>8</v>
+      </c>
+      <c r="Y7" s="4">
+        <f>SUM('Week 1 Total'!Y7,'Week 2 Total'!Y7,'Week 3 Total'!Y7,'Week 4 Total'!Y7)</f>
+        <v>8</v>
+      </c>
+      <c r="Z7" s="2">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="AA7" s="4">
+        <f>SUM('Week 1 Total'!AA7,'Week 2 Total'!AA7,'Week 3 Total'!AA7,'Week 4 Total'!AA7)</f>
+        <v>45</v>
+      </c>
+      <c r="AB7" s="4">
+        <f>SUM('Week 1 Total'!AB7,'Week 2 Total'!AB7,'Week 3 Total'!AB7,'Week 4 Total'!AB7)</f>
+        <v>18</v>
+      </c>
+      <c r="AC7" s="4">
+        <f>SUM('Week 1 Total'!AC7,'Week 2 Total'!AC7,'Week 3 Total'!AC7,'Week 4 Total'!AC7)</f>
+        <v>27</v>
+      </c>
+      <c r="AD7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="AE7" s="4">
+        <f>SUM('Week 1 Total'!AE7,'Week 2 Total'!AE7,'Week 3 Total'!AE7,'Week 4 Total'!AE7)</f>
+        <v>8</v>
+      </c>
+      <c r="AF7" s="4">
+        <f>SUM('Week 1 Total'!AF7,'Week 2 Total'!AF7,'Week 3 Total'!AF7,'Week 4 Total'!AF7)</f>
+        <v>6</v>
+      </c>
+      <c r="AG7" s="4">
+        <f>SUM('Week 1 Total'!AG7,'Week 2 Total'!AG7,'Week 3 Total'!AG7,'Week 4 Total'!AG7)</f>
+        <v>2</v>
+      </c>
+      <c r="AH7" s="2">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="AI7" s="4">
+        <f>SUM('Week 1 Total'!AI7,'Week 2 Total'!AI7,'Week 3 Total'!AI7,'Week 4 Total'!AI7)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="4">
+        <f>SUM('Week 1 Total'!AJ7,'Week 2 Total'!AJ7,'Week 3 Total'!AJ7,'Week 4 Total'!AJ7)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4">
+        <f>SUM('Week 1 Total'!C8,'Week 2 Total'!C8,'Week 3 Total'!C8,'Week 4 Total'!C8)</f>
+        <v>51</v>
+      </c>
+      <c r="D8" s="4">
+        <f>SUM('Week 1 Total'!D8,'Week 2 Total'!D8,'Week 3 Total'!D8,'Week 4 Total'!D8)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <f>SUM('Week 1 Total'!E8,'Week 2 Total'!E8,'Week 3 Total'!E8,'Week 4 Total'!E8)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <f>SUM('Week 1 Total'!F8,'Week 2 Total'!F8,'Week 3 Total'!F8,'Week 4 Total'!F8)</f>
+        <v>12</v>
+      </c>
+      <c r="G8" s="4">
+        <f>SUM('Week 1 Total'!G8,'Week 2 Total'!G8,'Week 3 Total'!G8,'Week 4 Total'!G8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <f>SUM('Week 1 Total'!H8,'Week 2 Total'!H8,'Week 3 Total'!H8,'Week 4 Total'!H8)</f>
+        <v>4</v>
+      </c>
+      <c r="I8" s="4">
+        <f>SUM('Week 1 Total'!I8,'Week 2 Total'!I8,'Week 3 Total'!I8,'Week 4 Total'!I8)</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K8" s="4">
+        <f>SUM('Week 1 Total'!K8,'Week 2 Total'!K8,'Week 3 Total'!K8,'Week 4 Total'!K8)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <f>SUM('Week 1 Total'!L8,'Week 2 Total'!L8,'Week 3 Total'!L8,'Week 4 Total'!L8)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <f>SUM('Week 1 Total'!M8,'Week 2 Total'!M8,'Week 3 Total'!M8,'Week 4 Total'!M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <f>SUM('Week 1 Total'!N8,'Week 2 Total'!N8,'Week 3 Total'!N8,'Week 4 Total'!N8)</f>
+        <v>6</v>
+      </c>
+      <c r="O8" s="4">
+        <f>SUM('Week 1 Total'!O8,'Week 2 Total'!O8,'Week 3 Total'!O8,'Week 4 Total'!O8)</f>
+        <v>2</v>
+      </c>
+      <c r="P8" s="4">
+        <f>SUM('Week 1 Total'!P8,'Week 2 Total'!P8,'Week 3 Total'!P8,'Week 4 Total'!P8)</f>
+        <v>4</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>SUM('Week 1 Total'!Q8,'Week 2 Total'!Q8,'Week 3 Total'!Q8,'Week 4 Total'!Q8)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="4">
+        <f>SUM('Week 1 Total'!R8,'Week 2 Total'!R8,'Week 3 Total'!R8,'Week 4 Total'!R8)</f>
+        <v>9</v>
+      </c>
+      <c r="S8" s="4">
+        <f>SUM('Week 1 Total'!S8,'Week 2 Total'!S8,'Week 3 Total'!S8,'Week 4 Total'!S8)</f>
+        <v>4</v>
+      </c>
+      <c r="T8" s="4">
+        <f>SUM('Week 1 Total'!T8,'Week 2 Total'!T8,'Week 3 Total'!T8,'Week 4 Total'!T8)</f>
+        <v>5</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4">
+        <f>SUM('Week 1 Total'!W8,'Week 2 Total'!W8,'Week 3 Total'!W8,'Week 4 Total'!W8)</f>
+        <v>2</v>
+      </c>
+      <c r="X8" s="4">
+        <f>SUM('Week 1 Total'!X8,'Week 2 Total'!X8,'Week 3 Total'!X8,'Week 4 Total'!X8)</f>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="4">
+        <f>SUM('Week 1 Total'!Y8,'Week 2 Total'!Y8,'Week 3 Total'!Y8,'Week 4 Total'!Y8)</f>
+        <v>2</v>
+      </c>
+      <c r="Z8" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="4">
+        <f>SUM('Week 1 Total'!AA8,'Week 2 Total'!AA8,'Week 3 Total'!AA8,'Week 4 Total'!AA8)</f>
+        <v>7</v>
+      </c>
+      <c r="AB8" s="4">
+        <f>SUM('Week 1 Total'!AB8,'Week 2 Total'!AB8,'Week 3 Total'!AB8,'Week 4 Total'!AB8)</f>
+        <v>4</v>
+      </c>
+      <c r="AC8" s="4">
+        <f>SUM('Week 1 Total'!AC8,'Week 2 Total'!AC8,'Week 3 Total'!AC8,'Week 4 Total'!AC8)</f>
+        <v>3</v>
+      </c>
+      <c r="AD8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="AE8" s="4">
+        <f>SUM('Week 1 Total'!AE8,'Week 2 Total'!AE8,'Week 3 Total'!AE8,'Week 4 Total'!AE8)</f>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="4">
+        <f>SUM('Week 1 Total'!AF8,'Week 2 Total'!AF8,'Week 3 Total'!AF8,'Week 4 Total'!AF8)</f>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="4">
+        <f>SUM('Week 1 Total'!AG8,'Week 2 Total'!AG8,'Week 3 Total'!AG8,'Week 4 Total'!AG8)</f>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="4">
+        <f>SUM('Week 1 Total'!AI8,'Week 2 Total'!AI8,'Week 3 Total'!AI8,'Week 4 Total'!AI8)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="4">
+        <f>SUM('Week 1 Total'!AJ8,'Week 2 Total'!AJ8,'Week 3 Total'!AJ8,'Week 4 Total'!AJ8)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4">
+        <f>SUM('Week 1 Total'!C9,'Week 2 Total'!C9,'Week 3 Total'!C9,'Week 4 Total'!C9)</f>
+        <v>198</v>
+      </c>
+      <c r="D9" s="4">
+        <f>SUM('Week 1 Total'!D9,'Week 2 Total'!D9,'Week 3 Total'!D9,'Week 4 Total'!D9)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <f>SUM('Week 1 Total'!E9,'Week 2 Total'!E9,'Week 3 Total'!E9,'Week 4 Total'!E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <f>SUM('Week 1 Total'!F9,'Week 2 Total'!F9,'Week 3 Total'!F9,'Week 4 Total'!F9)</f>
+        <v>75</v>
+      </c>
+      <c r="G9" s="4">
+        <f>SUM('Week 1 Total'!G9,'Week 2 Total'!G9,'Week 3 Total'!G9,'Week 4 Total'!G9)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f>SUM('Week 1 Total'!H9,'Week 2 Total'!H9,'Week 3 Total'!H9,'Week 4 Total'!H9)</f>
+        <v>8</v>
+      </c>
+      <c r="I9" s="4">
+        <f>SUM('Week 1 Total'!I9,'Week 2 Total'!I9,'Week 3 Total'!I9,'Week 4 Total'!I9)</f>
+        <v>3</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="1"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="K9" s="4">
+        <f>SUM('Week 1 Total'!K9,'Week 2 Total'!K9,'Week 3 Total'!K9,'Week 4 Total'!K9)</f>
+        <v>7</v>
+      </c>
+      <c r="L9" s="4">
+        <f>SUM('Week 1 Total'!L9,'Week 2 Total'!L9,'Week 3 Total'!L9,'Week 4 Total'!L9)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <f>SUM('Week 1 Total'!M9,'Week 2 Total'!M9,'Week 3 Total'!M9,'Week 4 Total'!M9)</f>
+        <v>2</v>
+      </c>
+      <c r="N9" s="4">
+        <f>SUM('Week 1 Total'!N9,'Week 2 Total'!N9,'Week 3 Total'!N9,'Week 4 Total'!N9)</f>
+        <v>75</v>
+      </c>
+      <c r="O9" s="4">
+        <f>SUM('Week 1 Total'!O9,'Week 2 Total'!O9,'Week 3 Total'!O9,'Week 4 Total'!O9)</f>
+        <v>25</v>
+      </c>
+      <c r="P9" s="4">
+        <f>SUM('Week 1 Total'!P9,'Week 2 Total'!P9,'Week 3 Total'!P9,'Week 4 Total'!P9)</f>
+        <v>50</v>
+      </c>
+      <c r="Q9" s="4">
+        <f>SUM('Week 1 Total'!Q9,'Week 2 Total'!Q9,'Week 3 Total'!Q9,'Week 4 Total'!Q9)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <f>SUM('Week 1 Total'!R9,'Week 2 Total'!R9,'Week 3 Total'!R9,'Week 4 Total'!R9)</f>
+        <v>61</v>
+      </c>
+      <c r="S9" s="4">
+        <f>SUM('Week 1 Total'!S9,'Week 2 Total'!S9,'Week 3 Total'!S9,'Week 4 Total'!S9)</f>
+        <v>33</v>
+      </c>
+      <c r="T9" s="4">
+        <f>SUM('Week 1 Total'!T9,'Week 2 Total'!T9,'Week 3 Total'!T9,'Week 4 Total'!T9)</f>
+        <v>28</v>
+      </c>
+      <c r="U9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.54098360655737709</v>
+      </c>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4">
+        <f>SUM('Week 1 Total'!W9,'Week 2 Total'!W9,'Week 3 Total'!W9,'Week 4 Total'!W9)</f>
+        <v>61</v>
+      </c>
+      <c r="X9" s="4">
+        <f>SUM('Week 1 Total'!X9,'Week 2 Total'!X9,'Week 3 Total'!X9,'Week 4 Total'!X9)</f>
+        <v>33</v>
+      </c>
+      <c r="Y9" s="4">
+        <f>SUM('Week 1 Total'!Y9,'Week 2 Total'!Y9,'Week 3 Total'!Y9,'Week 4 Total'!Y9)</f>
+        <v>28</v>
+      </c>
+      <c r="Z9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.54098360655737709</v>
+      </c>
+      <c r="AA9" s="4">
+        <f>SUM('Week 1 Total'!AA9,'Week 2 Total'!AA9,'Week 3 Total'!AA9,'Week 4 Total'!AA9)</f>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="4">
+        <f>SUM('Week 1 Total'!AB9,'Week 2 Total'!AB9,'Week 3 Total'!AB9,'Week 4 Total'!AB9)</f>
+        <v>0</v>
+      </c>
+      <c r="AC9" s="4">
+        <f>SUM('Week 1 Total'!AC9,'Week 2 Total'!AC9,'Week 3 Total'!AC9,'Week 4 Total'!AC9)</f>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE9" s="4">
+        <f>SUM('Week 1 Total'!AE9,'Week 2 Total'!AE9,'Week 3 Total'!AE9,'Week 4 Total'!AE9)</f>
+        <v>15</v>
+      </c>
+      <c r="AF9" s="4">
+        <f>SUM('Week 1 Total'!AF9,'Week 2 Total'!AF9,'Week 3 Total'!AF9,'Week 4 Total'!AF9)</f>
+        <v>9</v>
+      </c>
+      <c r="AG9" s="4">
+        <f>SUM('Week 1 Total'!AG9,'Week 2 Total'!AG9,'Week 3 Total'!AG9,'Week 4 Total'!AG9)</f>
+        <v>6</v>
+      </c>
+      <c r="AH9" s="2">
+        <f t="shared" si="4"/>
+        <v>0.6</v>
+      </c>
+      <c r="AI9" s="4">
+        <f>SUM('Week 1 Total'!AI9,'Week 2 Total'!AI9,'Week 3 Total'!AI9,'Week 4 Total'!AI9)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ9" s="4">
+        <f>SUM('Week 1 Total'!AJ9,'Week 2 Total'!AJ9,'Week 3 Total'!AJ9,'Week 4 Total'!AJ9)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="4">
+        <f>SUM('Week 1 Total'!C10,'Week 2 Total'!C10,'Week 3 Total'!C10,'Week 4 Total'!C10)</f>
+        <v>249</v>
+      </c>
+      <c r="D10" s="4">
+        <f>SUM('Week 1 Total'!D10,'Week 2 Total'!D10,'Week 3 Total'!D10,'Week 4 Total'!D10)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <f>SUM('Week 1 Total'!E10,'Week 2 Total'!E10,'Week 3 Total'!E10,'Week 4 Total'!E10)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <f>SUM('Week 1 Total'!F10,'Week 2 Total'!F10,'Week 3 Total'!F10,'Week 4 Total'!F10)</f>
+        <v>138</v>
+      </c>
+      <c r="G10" s="4">
+        <f>SUM('Week 1 Total'!G10,'Week 2 Total'!G10,'Week 3 Total'!G10,'Week 4 Total'!G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <f>SUM('Week 1 Total'!H10,'Week 2 Total'!H10,'Week 3 Total'!H10,'Week 4 Total'!H10)</f>
+        <v>18</v>
+      </c>
+      <c r="I10" s="4">
+        <f>SUM('Week 1 Total'!I10,'Week 2 Total'!I10,'Week 3 Total'!I10,'Week 4 Total'!I10)</f>
+        <v>18</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
+        <f>SUM('Week 1 Total'!K10,'Week 2 Total'!K10,'Week 3 Total'!K10,'Week 4 Total'!K10)</f>
+        <v>12</v>
+      </c>
+      <c r="L10" s="4">
+        <f>SUM('Week 1 Total'!L10,'Week 2 Total'!L10,'Week 3 Total'!L10,'Week 4 Total'!L10)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <f>SUM('Week 1 Total'!M10,'Week 2 Total'!M10,'Week 3 Total'!M10,'Week 4 Total'!M10)</f>
+        <v>2</v>
+      </c>
+      <c r="N10" s="4">
+        <f>SUM('Week 1 Total'!N10,'Week 2 Total'!N10,'Week 3 Total'!N10,'Week 4 Total'!N10)</f>
+        <v>26</v>
+      </c>
+      <c r="O10" s="4">
+        <f>SUM('Week 1 Total'!O10,'Week 2 Total'!O10,'Week 3 Total'!O10,'Week 4 Total'!O10)</f>
+        <v>6</v>
+      </c>
+      <c r="P10" s="4">
+        <f>SUM('Week 1 Total'!P10,'Week 2 Total'!P10,'Week 3 Total'!P10,'Week 4 Total'!P10)</f>
+        <v>20</v>
+      </c>
+      <c r="Q10" s="4">
+        <f>SUM('Week 1 Total'!Q10,'Week 2 Total'!Q10,'Week 3 Total'!Q10,'Week 4 Total'!Q10)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="4">
+        <f>SUM('Week 1 Total'!R10,'Week 2 Total'!R10,'Week 3 Total'!R10,'Week 4 Total'!R10)</f>
+        <v>104</v>
+      </c>
+      <c r="S10" s="4">
+        <f>SUM('Week 1 Total'!S10,'Week 2 Total'!S10,'Week 3 Total'!S10,'Week 4 Total'!S10)</f>
+        <v>49</v>
+      </c>
+      <c r="T10" s="4">
+        <f>SUM('Week 1 Total'!T10,'Week 2 Total'!T10,'Week 3 Total'!T10,'Week 4 Total'!T10)</f>
+        <v>55</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.47115384615384615</v>
+      </c>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4">
+        <f>SUM('Week 1 Total'!W10,'Week 2 Total'!W10,'Week 3 Total'!W10,'Week 4 Total'!W10)</f>
+        <v>57</v>
+      </c>
+      <c r="X10" s="4">
+        <f>SUM('Week 1 Total'!X10,'Week 2 Total'!X10,'Week 3 Total'!X10,'Week 4 Total'!X10)</f>
+        <v>31</v>
+      </c>
+      <c r="Y10" s="4">
+        <f>SUM('Week 1 Total'!Y10,'Week 2 Total'!Y10,'Week 3 Total'!Y10,'Week 4 Total'!Y10)</f>
+        <v>26</v>
+      </c>
+      <c r="Z10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.54385964912280704</v>
+      </c>
+      <c r="AA10" s="4">
+        <f>SUM('Week 1 Total'!AA10,'Week 2 Total'!AA10,'Week 3 Total'!AA10,'Week 4 Total'!AA10)</f>
+        <v>47</v>
+      </c>
+      <c r="AB10" s="4">
+        <f>SUM('Week 1 Total'!AB10,'Week 2 Total'!AB10,'Week 3 Total'!AB10,'Week 4 Total'!AB10)</f>
+        <v>18</v>
+      </c>
+      <c r="AC10" s="4">
+        <f>SUM('Week 1 Total'!AC10,'Week 2 Total'!AC10,'Week 3 Total'!AC10,'Week 4 Total'!AC10)</f>
+        <v>29</v>
+      </c>
+      <c r="AD10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.38297872340425532</v>
+      </c>
+      <c r="AE10" s="4">
+        <f>SUM('Week 1 Total'!AE10,'Week 2 Total'!AE10,'Week 3 Total'!AE10,'Week 4 Total'!AE10)</f>
+        <v>28</v>
+      </c>
+      <c r="AF10" s="4">
+        <f>SUM('Week 1 Total'!AF10,'Week 2 Total'!AF10,'Week 3 Total'!AF10,'Week 4 Total'!AF10)</f>
+        <v>22</v>
+      </c>
+      <c r="AG10" s="4">
+        <f>SUM('Week 1 Total'!AG10,'Week 2 Total'!AG10,'Week 3 Total'!AG10,'Week 4 Total'!AG10)</f>
+        <v>6</v>
+      </c>
+      <c r="AH10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="AI10" s="4">
+        <f>SUM('Week 1 Total'!AI10,'Week 2 Total'!AI10,'Week 3 Total'!AI10,'Week 4 Total'!AI10)</f>
+        <v>4</v>
+      </c>
+      <c r="AJ10" s="4">
+        <f>SUM('Week 1 Total'!AJ10,'Week 2 Total'!AJ10,'Week 3 Total'!AJ10,'Week 4 Total'!AJ10)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="4">
+        <f>SUM('Week 1 Total'!C11,'Week 2 Total'!C11,'Week 3 Total'!C11,'Week 4 Total'!C11)</f>
+        <v>11</v>
+      </c>
+      <c r="D11" s="4">
+        <f>SUM('Week 1 Total'!D11,'Week 2 Total'!D11,'Week 3 Total'!D11,'Week 4 Total'!D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <f>SUM('Week 1 Total'!E11,'Week 2 Total'!E11,'Week 3 Total'!E11,'Week 4 Total'!E11)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <f>SUM('Week 1 Total'!F11,'Week 2 Total'!F11,'Week 3 Total'!F11,'Week 4 Total'!F11)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <f>SUM('Week 1 Total'!G11,'Week 2 Total'!G11,'Week 3 Total'!G11,'Week 4 Total'!G11)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <f>SUM('Week 1 Total'!H11,'Week 2 Total'!H11,'Week 3 Total'!H11,'Week 4 Total'!H11)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <f>SUM('Week 1 Total'!I11,'Week 2 Total'!I11,'Week 3 Total'!I11,'Week 4 Total'!I11)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="K11" s="4">
+        <f>SUM('Week 1 Total'!K11,'Week 2 Total'!K11,'Week 3 Total'!K11,'Week 4 Total'!K11)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <f>SUM('Week 1 Total'!L11,'Week 2 Total'!L11,'Week 3 Total'!L11,'Week 4 Total'!L11)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <f>SUM('Week 1 Total'!M11,'Week 2 Total'!M11,'Week 3 Total'!M11,'Week 4 Total'!M11)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <f>SUM('Week 1 Total'!N11,'Week 2 Total'!N11,'Week 3 Total'!N11,'Week 4 Total'!N11)</f>
+        <v>1</v>
+      </c>
+      <c r="O11" s="4">
+        <f>SUM('Week 1 Total'!O11,'Week 2 Total'!O11,'Week 3 Total'!O11,'Week 4 Total'!O11)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <f>SUM('Week 1 Total'!P11,'Week 2 Total'!P11,'Week 3 Total'!P11,'Week 4 Total'!P11)</f>
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4">
+        <f>SUM('Week 1 Total'!Q11,'Week 2 Total'!Q11,'Week 3 Total'!Q11,'Week 4 Total'!Q11)</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="4">
+        <f>SUM('Week 1 Total'!R11,'Week 2 Total'!R11,'Week 3 Total'!R11,'Week 4 Total'!R11)</f>
+        <v>2</v>
+      </c>
+      <c r="S11" s="4">
+        <f>SUM('Week 1 Total'!S11,'Week 2 Total'!S11,'Week 3 Total'!S11,'Week 4 Total'!S11)</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="4">
+        <f>SUM('Week 1 Total'!T11,'Week 2 Total'!T11,'Week 3 Total'!T11,'Week 4 Total'!T11)</f>
+        <v>2</v>
+      </c>
+      <c r="U11" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4">
+        <f>SUM('Week 1 Total'!W11,'Week 2 Total'!W11,'Week 3 Total'!W11,'Week 4 Total'!W11)</f>
+        <v>1</v>
+      </c>
+      <c r="X11" s="4">
+        <f>SUM('Week 1 Total'!X11,'Week 2 Total'!X11,'Week 3 Total'!X11,'Week 4 Total'!X11)</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="4">
+        <f>SUM('Week 1 Total'!Y11,'Week 2 Total'!Y11,'Week 3 Total'!Y11,'Week 4 Total'!Y11)</f>
+        <v>1</v>
+      </c>
+      <c r="Z11" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="4">
+        <f>SUM('Week 1 Total'!AA11,'Week 2 Total'!AA11,'Week 3 Total'!AA11,'Week 4 Total'!AA11)</f>
+        <v>1</v>
+      </c>
+      <c r="AB11" s="4">
+        <f>SUM('Week 1 Total'!AB11,'Week 2 Total'!AB11,'Week 3 Total'!AB11,'Week 4 Total'!AB11)</f>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="4">
+        <f>SUM('Week 1 Total'!AC11,'Week 2 Total'!AC11,'Week 3 Total'!AC11,'Week 4 Total'!AC11)</f>
+        <v>1</v>
+      </c>
+      <c r="AD11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE11" s="4">
+        <f>SUM('Week 1 Total'!AE11,'Week 2 Total'!AE11,'Week 3 Total'!AE11,'Week 4 Total'!AE11)</f>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="4">
+        <f>SUM('Week 1 Total'!AF11,'Week 2 Total'!AF11,'Week 3 Total'!AF11,'Week 4 Total'!AF11)</f>
+        <v>0</v>
+      </c>
+      <c r="AG11" s="4">
+        <f>SUM('Week 1 Total'!AG11,'Week 2 Total'!AG11,'Week 3 Total'!AG11,'Week 4 Total'!AG11)</f>
+        <v>0</v>
+      </c>
+      <c r="AH11" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AI11" s="4">
+        <f>SUM('Week 1 Total'!AI11,'Week 2 Total'!AI11,'Week 3 Total'!AI11,'Week 4 Total'!AI11)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="4">
+        <f>SUM('Week 1 Total'!AJ11,'Week 2 Total'!AJ11,'Week 3 Total'!AJ11,'Week 4 Total'!AJ11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="4">
+        <f>SUM('Week 1 Total'!C12,'Week 2 Total'!C12,'Week 3 Total'!C12,'Week 4 Total'!C12)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <f>SUM('Week 1 Total'!D12,'Week 2 Total'!D12,'Week 3 Total'!D12,'Week 4 Total'!D12)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <f>SUM('Week 1 Total'!E12,'Week 2 Total'!E12,'Week 3 Total'!E12,'Week 4 Total'!E12)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <f>SUM('Week 1 Total'!F12,'Week 2 Total'!F12,'Week 3 Total'!F12,'Week 4 Total'!F12)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <f>SUM('Week 1 Total'!G12,'Week 2 Total'!G12,'Week 3 Total'!G12,'Week 4 Total'!G12)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <f>SUM('Week 1 Total'!H12,'Week 2 Total'!H12,'Week 3 Total'!H12,'Week 4 Total'!H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <f>SUM('Week 1 Total'!I12,'Week 2 Total'!I12,'Week 3 Total'!I12,'Week 4 Total'!I12)</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="K12" s="4">
+        <f>SUM('Week 1 Total'!K12,'Week 2 Total'!K12,'Week 3 Total'!K12,'Week 4 Total'!K12)</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <f>SUM('Week 1 Total'!L12,'Week 2 Total'!L12,'Week 3 Total'!L12,'Week 4 Total'!L12)</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <f>SUM('Week 1 Total'!M12,'Week 2 Total'!M12,'Week 3 Total'!M12,'Week 4 Total'!M12)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <f>SUM('Week 1 Total'!N12,'Week 2 Total'!N12,'Week 3 Total'!N12,'Week 4 Total'!N12)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <f>SUM('Week 1 Total'!O12,'Week 2 Total'!O12,'Week 3 Total'!O12,'Week 4 Total'!O12)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <f>SUM('Week 1 Total'!P12,'Week 2 Total'!P12,'Week 3 Total'!P12,'Week 4 Total'!P12)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4">
+        <f>SUM('Week 1 Total'!Q12,'Week 2 Total'!Q12,'Week 3 Total'!Q12,'Week 4 Total'!Q12)</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <f>SUM('Week 1 Total'!R12,'Week 2 Total'!R12,'Week 3 Total'!R12,'Week 4 Total'!R12)</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="4">
+        <f>SUM('Week 1 Total'!S12,'Week 2 Total'!S12,'Week 3 Total'!S12,'Week 4 Total'!S12)</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="4">
+        <f>SUM('Week 1 Total'!T12,'Week 2 Total'!T12,'Week 3 Total'!T12,'Week 4 Total'!T12)</f>
+        <v>0</v>
+      </c>
+      <c r="U12" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4">
+        <f>SUM('Week 1 Total'!W12,'Week 2 Total'!W12,'Week 3 Total'!W12,'Week 4 Total'!W12)</f>
+        <v>0</v>
+      </c>
+      <c r="X12" s="4">
+        <f>SUM('Week 1 Total'!X12,'Week 2 Total'!X12,'Week 3 Total'!X12,'Week 4 Total'!X12)</f>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="4">
+        <f>SUM('Week 1 Total'!Y12,'Week 2 Total'!Y12,'Week 3 Total'!Y12,'Week 4 Total'!Y12)</f>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="4">
+        <f>SUM('Week 1 Total'!AA12,'Week 2 Total'!AA12,'Week 3 Total'!AA12,'Week 4 Total'!AA12)</f>
+        <v>0</v>
+      </c>
+      <c r="AB12" s="4">
+        <f>SUM('Week 1 Total'!AB12,'Week 2 Total'!AB12,'Week 3 Total'!AB12,'Week 4 Total'!AB12)</f>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="4">
+        <f>SUM('Week 1 Total'!AC12,'Week 2 Total'!AC12,'Week 3 Total'!AC12,'Week 4 Total'!AC12)</f>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="2">
+        <f>IF(ISERROR(AB12/AA12),0,AB12/AA12)</f>
+        <v>0</v>
+      </c>
+      <c r="AE12" s="4">
+        <f>SUM('Week 1 Total'!AE12,'Week 2 Total'!AE12,'Week 3 Total'!AE12,'Week 4 Total'!AE12)</f>
+        <v>0</v>
+      </c>
+      <c r="AF12" s="4">
+        <f>SUM('Week 1 Total'!AF12,'Week 2 Total'!AF12,'Week 3 Total'!AF12,'Week 4 Total'!AF12)</f>
+        <v>0</v>
+      </c>
+      <c r="AG12" s="4">
+        <f>SUM('Week 1 Total'!AG12,'Week 2 Total'!AG12,'Week 3 Total'!AG12,'Week 4 Total'!AG12)</f>
+        <v>0</v>
+      </c>
+      <c r="AH12" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AI12" s="4">
+        <f>SUM('Week 1 Total'!AI12,'Week 2 Total'!AI12,'Week 3 Total'!AI12,'Week 4 Total'!AI12)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="4">
+        <f>SUM('Week 1 Total'!AJ12,'Week 2 Total'!AJ12,'Week 3 Total'!AJ12,'Week 4 Total'!AJ12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4">
+        <f>SUM('Week 1 Total'!C13,'Week 2 Total'!C13,'Week 3 Total'!C13,'Week 4 Total'!C13)</f>
+        <v>113</v>
+      </c>
+      <c r="D13" s="4">
+        <f>SUM('Week 1 Total'!D13,'Week 2 Total'!D13,'Week 3 Total'!D13,'Week 4 Total'!D13)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <f>SUM('Week 1 Total'!E13,'Week 2 Total'!E13,'Week 3 Total'!E13,'Week 4 Total'!E13)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <f>SUM('Week 1 Total'!F13,'Week 2 Total'!F13,'Week 3 Total'!F13,'Week 4 Total'!F13)</f>
+        <v>31</v>
+      </c>
+      <c r="G13" s="4">
+        <f>SUM('Week 1 Total'!G13,'Week 2 Total'!G13,'Week 3 Total'!G13,'Week 4 Total'!G13)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <f>SUM('Week 1 Total'!H13,'Week 2 Total'!H13,'Week 3 Total'!H13,'Week 4 Total'!H13)</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="4">
+        <f>SUM('Week 1 Total'!I13,'Week 2 Total'!I13,'Week 3 Total'!I13,'Week 4 Total'!I13)</f>
+        <v>11</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="1"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="K13" s="4">
+        <f>SUM('Week 1 Total'!K13,'Week 2 Total'!K13,'Week 3 Total'!K13,'Week 4 Total'!K13)</f>
+        <v>3</v>
+      </c>
+      <c r="L13" s="4">
+        <f>SUM('Week 1 Total'!L13,'Week 2 Total'!L13,'Week 3 Total'!L13,'Week 4 Total'!L13)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <f>SUM('Week 1 Total'!M13,'Week 2 Total'!M13,'Week 3 Total'!M13,'Week 4 Total'!M13)</f>
+        <v>21</v>
+      </c>
+      <c r="N13" s="4">
+        <f>SUM('Week 1 Total'!N13,'Week 2 Total'!N13,'Week 3 Total'!N13,'Week 4 Total'!N13)</f>
+        <v>23</v>
+      </c>
+      <c r="O13" s="4">
+        <f>SUM('Week 1 Total'!O13,'Week 2 Total'!O13,'Week 3 Total'!O13,'Week 4 Total'!O13)</f>
+        <v>5</v>
+      </c>
+      <c r="P13" s="4">
+        <f>SUM('Week 1 Total'!P13,'Week 2 Total'!P13,'Week 3 Total'!P13,'Week 4 Total'!P13)</f>
+        <v>18</v>
+      </c>
+      <c r="Q13" s="4">
+        <f>SUM('Week 1 Total'!Q13,'Week 2 Total'!Q13,'Week 3 Total'!Q13,'Week 4 Total'!Q13)</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="4">
+        <f>SUM('Week 1 Total'!R13,'Week 2 Total'!R13,'Week 3 Total'!R13,'Week 4 Total'!R13)</f>
+        <v>20</v>
+      </c>
+      <c r="S13" s="4">
+        <f>SUM('Week 1 Total'!S13,'Week 2 Total'!S13,'Week 3 Total'!S13,'Week 4 Total'!S13)</f>
+        <v>14</v>
+      </c>
+      <c r="T13" s="4">
+        <f>SUM('Week 1 Total'!T13,'Week 2 Total'!T13,'Week 3 Total'!T13,'Week 4 Total'!T13)</f>
+        <v>6</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4">
+        <f>SUM('Week 1 Total'!W13,'Week 2 Total'!W13,'Week 3 Total'!W13,'Week 4 Total'!W13)</f>
+        <v>20</v>
+      </c>
+      <c r="X13" s="4">
+        <f>SUM('Week 1 Total'!X13,'Week 2 Total'!X13,'Week 3 Total'!X13,'Week 4 Total'!X13)</f>
+        <v>14</v>
+      </c>
+      <c r="Y13" s="4">
+        <f>SUM('Week 1 Total'!Y13,'Week 2 Total'!Y13,'Week 3 Total'!Y13,'Week 4 Total'!Y13)</f>
+        <v>6</v>
+      </c>
+      <c r="Z13" s="2">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="AA13" s="4">
+        <f>SUM('Week 1 Total'!AA13,'Week 2 Total'!AA13,'Week 3 Total'!AA13,'Week 4 Total'!AA13)</f>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="4">
+        <f>SUM('Week 1 Total'!AB13,'Week 2 Total'!AB13,'Week 3 Total'!AB13,'Week 4 Total'!AB13)</f>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="4">
+        <f>SUM('Week 1 Total'!AC13,'Week 2 Total'!AC13,'Week 3 Total'!AC13,'Week 4 Total'!AC13)</f>
+        <v>0</v>
+      </c>
+      <c r="AD13" s="2">
+        <f t="shared" ref="AD13:AD17" si="5">IF(ISERROR(AB13/AA13),0,AB13/AA13)</f>
+        <v>0</v>
+      </c>
+      <c r="AE13" s="4">
+        <f>SUM('Week 1 Total'!AE13,'Week 2 Total'!AE13,'Week 3 Total'!AE13,'Week 4 Total'!AE13)</f>
+        <v>4</v>
+      </c>
+      <c r="AF13" s="4">
+        <f>SUM('Week 1 Total'!AF13,'Week 2 Total'!AF13,'Week 3 Total'!AF13,'Week 4 Total'!AF13)</f>
+        <v>3</v>
+      </c>
+      <c r="AG13" s="4">
+        <f>SUM('Week 1 Total'!AG13,'Week 2 Total'!AG13,'Week 3 Total'!AG13,'Week 4 Total'!AG13)</f>
+        <v>1</v>
+      </c>
+      <c r="AH13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="AI13" s="4">
+        <f>SUM('Week 1 Total'!AI13,'Week 2 Total'!AI13,'Week 3 Total'!AI13,'Week 4 Total'!AI13)</f>
+        <v>2</v>
+      </c>
+      <c r="AJ13" s="4">
+        <f>SUM('Week 1 Total'!AJ13,'Week 2 Total'!AJ13,'Week 3 Total'!AJ13,'Week 4 Total'!AJ13)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4">
+        <f>SUM('Week 1 Total'!C14,'Week 2 Total'!C14,'Week 3 Total'!C14,'Week 4 Total'!C14)</f>
+        <v>5</v>
+      </c>
+      <c r="D14" s="4">
+        <f>SUM('Week 1 Total'!D14,'Week 2 Total'!D14,'Week 3 Total'!D14,'Week 4 Total'!D14)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <f>SUM('Week 1 Total'!E14,'Week 2 Total'!E14,'Week 3 Total'!E14,'Week 4 Total'!E14)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <f>SUM('Week 1 Total'!F14,'Week 2 Total'!F14,'Week 3 Total'!F14,'Week 4 Total'!F14)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <f>SUM('Week 1 Total'!G14,'Week 2 Total'!G14,'Week 3 Total'!G14,'Week 4 Total'!G14)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <f>SUM('Week 1 Total'!H14,'Week 2 Total'!H14,'Week 3 Total'!H14,'Week 4 Total'!H14)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <f>SUM('Week 1 Total'!I14,'Week 2 Total'!I14,'Week 3 Total'!I14,'Week 4 Total'!I14)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="K14" s="4">
+        <f>SUM('Week 1 Total'!K14,'Week 2 Total'!K14,'Week 3 Total'!K14,'Week 4 Total'!K14)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <f>SUM('Week 1 Total'!L14,'Week 2 Total'!L14,'Week 3 Total'!L14,'Week 4 Total'!L14)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <f>SUM('Week 1 Total'!M14,'Week 2 Total'!M14,'Week 3 Total'!M14,'Week 4 Total'!M14)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <f>SUM('Week 1 Total'!N14,'Week 2 Total'!N14,'Week 3 Total'!N14,'Week 4 Total'!N14)</f>
+        <v>1</v>
+      </c>
+      <c r="O14" s="4">
+        <f>SUM('Week 1 Total'!O14,'Week 2 Total'!O14,'Week 3 Total'!O14,'Week 4 Total'!O14)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <f>SUM('Week 1 Total'!P14,'Week 2 Total'!P14,'Week 3 Total'!P14,'Week 4 Total'!P14)</f>
+        <v>1</v>
+      </c>
+      <c r="Q14" s="4">
+        <f>SUM('Week 1 Total'!Q14,'Week 2 Total'!Q14,'Week 3 Total'!Q14,'Week 4 Total'!Q14)</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="4">
+        <f>SUM('Week 1 Total'!R14,'Week 2 Total'!R14,'Week 3 Total'!R14,'Week 4 Total'!R14)</f>
+        <v>2</v>
+      </c>
+      <c r="S14" s="4">
+        <f>SUM('Week 1 Total'!S14,'Week 2 Total'!S14,'Week 3 Total'!S14,'Week 4 Total'!S14)</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="4">
+        <f>SUM('Week 1 Total'!T14,'Week 2 Total'!T14,'Week 3 Total'!T14,'Week 4 Total'!T14)</f>
+        <v>2</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4">
+        <f>SUM('Week 1 Total'!W14,'Week 2 Total'!W14,'Week 3 Total'!W14,'Week 4 Total'!W14)</f>
+        <v>1</v>
+      </c>
+      <c r="X14" s="4">
+        <f>SUM('Week 1 Total'!X14,'Week 2 Total'!X14,'Week 3 Total'!X14,'Week 4 Total'!X14)</f>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="4">
+        <f>SUM('Week 1 Total'!Y14,'Week 2 Total'!Y14,'Week 3 Total'!Y14,'Week 4 Total'!Y14)</f>
+        <v>1</v>
+      </c>
+      <c r="Z14" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="4">
+        <f>SUM('Week 1 Total'!AA14,'Week 2 Total'!AA14,'Week 3 Total'!AA14,'Week 4 Total'!AA14)</f>
+        <v>1</v>
+      </c>
+      <c r="AB14" s="4">
+        <f>SUM('Week 1 Total'!AB14,'Week 2 Total'!AB14,'Week 3 Total'!AB14,'Week 4 Total'!AB14)</f>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="4">
+        <f>SUM('Week 1 Total'!AC14,'Week 2 Total'!AC14,'Week 3 Total'!AC14,'Week 4 Total'!AC14)</f>
+        <v>1</v>
+      </c>
+      <c r="AD14" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE14" s="4">
+        <f>SUM('Week 1 Total'!AE14,'Week 2 Total'!AE14,'Week 3 Total'!AE14,'Week 4 Total'!AE14)</f>
+        <v>0</v>
+      </c>
+      <c r="AF14" s="4">
+        <f>SUM('Week 1 Total'!AF14,'Week 2 Total'!AF14,'Week 3 Total'!AF14,'Week 4 Total'!AF14)</f>
+        <v>0</v>
+      </c>
+      <c r="AG14" s="4">
+        <f>SUM('Week 1 Total'!AG14,'Week 2 Total'!AG14,'Week 3 Total'!AG14,'Week 4 Total'!AG14)</f>
+        <v>0</v>
+      </c>
+      <c r="AH14" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AI14" s="4">
+        <f>SUM('Week 1 Total'!AI14,'Week 2 Total'!AI14,'Week 3 Total'!AI14,'Week 4 Total'!AI14)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="4">
+        <f>SUM('Week 1 Total'!AJ14,'Week 2 Total'!AJ14,'Week 3 Total'!AJ14,'Week 4 Total'!AJ14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="4">
+        <f>SUM('Week 1 Total'!C15,'Week 2 Total'!C15,'Week 3 Total'!C15,'Week 4 Total'!C15)</f>
+        <v>75</v>
+      </c>
+      <c r="D15" s="4">
+        <f>SUM('Week 1 Total'!D15,'Week 2 Total'!D15,'Week 3 Total'!D15,'Week 4 Total'!D15)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <f>SUM('Week 1 Total'!E15,'Week 2 Total'!E15,'Week 3 Total'!E15,'Week 4 Total'!E15)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <f>SUM('Week 1 Total'!F15,'Week 2 Total'!F15,'Week 3 Total'!F15,'Week 4 Total'!F15)</f>
+        <v>36</v>
+      </c>
+      <c r="G15" s="4">
+        <f>SUM('Week 1 Total'!G15,'Week 2 Total'!G15,'Week 3 Total'!G15,'Week 4 Total'!G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <f>SUM('Week 1 Total'!H15,'Week 2 Total'!H15,'Week 3 Total'!H15,'Week 4 Total'!H15)</f>
+        <v>3</v>
+      </c>
+      <c r="I15" s="4">
+        <f>SUM('Week 1 Total'!I15,'Week 2 Total'!I15,'Week 3 Total'!I15,'Week 4 Total'!I15)</f>
+        <v>10</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="K15" s="4">
+        <f>SUM('Week 1 Total'!K15,'Week 2 Total'!K15,'Week 3 Total'!K15,'Week 4 Total'!K15)</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <f>SUM('Week 1 Total'!L15,'Week 2 Total'!L15,'Week 3 Total'!L15,'Week 4 Total'!L15)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <f>SUM('Week 1 Total'!M15,'Week 2 Total'!M15,'Week 3 Total'!M15,'Week 4 Total'!M15)</f>
+        <v>9</v>
+      </c>
+      <c r="N15" s="4">
+        <f>SUM('Week 1 Total'!N15,'Week 2 Total'!N15,'Week 3 Total'!N15,'Week 4 Total'!N15)</f>
+        <v>17</v>
+      </c>
+      <c r="O15" s="4">
+        <f>SUM('Week 1 Total'!O15,'Week 2 Total'!O15,'Week 3 Total'!O15,'Week 4 Total'!O15)</f>
+        <v>7</v>
+      </c>
+      <c r="P15" s="4">
+        <f>SUM('Week 1 Total'!P15,'Week 2 Total'!P15,'Week 3 Total'!P15,'Week 4 Total'!P15)</f>
+        <v>10</v>
+      </c>
+      <c r="Q15" s="4">
+        <f>SUM('Week 1 Total'!Q15,'Week 2 Total'!Q15,'Week 3 Total'!Q15,'Week 4 Total'!Q15)</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="4">
+        <f>SUM('Week 1 Total'!R15,'Week 2 Total'!R15,'Week 3 Total'!R15,'Week 4 Total'!R15)</f>
+        <v>29</v>
+      </c>
+      <c r="S15" s="4">
+        <f>SUM('Week 1 Total'!S15,'Week 2 Total'!S15,'Week 3 Total'!S15,'Week 4 Total'!S15)</f>
+        <v>14</v>
+      </c>
+      <c r="T15" s="4">
+        <f>SUM('Week 1 Total'!T15,'Week 2 Total'!T15,'Week 3 Total'!T15,'Week 4 Total'!T15)</f>
+        <v>15</v>
+      </c>
+      <c r="U15" s="2">
+        <f t="shared" si="2"/>
+        <v>0.48275862068965519</v>
+      </c>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4">
+        <f>SUM('Week 1 Total'!W15,'Week 2 Total'!W15,'Week 3 Total'!W15,'Week 4 Total'!W15)</f>
+        <v>18</v>
+      </c>
+      <c r="X15" s="4">
+        <f>SUM('Week 1 Total'!X15,'Week 2 Total'!X15,'Week 3 Total'!X15,'Week 4 Total'!X15)</f>
+        <v>10</v>
+      </c>
+      <c r="Y15" s="4">
+        <f>SUM('Week 1 Total'!Y15,'Week 2 Total'!Y15,'Week 3 Total'!Y15,'Week 4 Total'!Y15)</f>
+        <v>8</v>
+      </c>
+      <c r="Z15" s="2">
+        <f t="shared" si="3"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="AA15" s="4">
+        <f>SUM('Week 1 Total'!AA15,'Week 2 Total'!AA15,'Week 3 Total'!AA15,'Week 4 Total'!AA15)</f>
+        <v>11</v>
+      </c>
+      <c r="AB15" s="4">
+        <f>SUM('Week 1 Total'!AB15,'Week 2 Total'!AB15,'Week 3 Total'!AB15,'Week 4 Total'!AB15)</f>
+        <v>4</v>
+      </c>
+      <c r="AC15" s="4">
+        <f>SUM('Week 1 Total'!AC15,'Week 2 Total'!AC15,'Week 3 Total'!AC15,'Week 4 Total'!AC15)</f>
+        <v>7</v>
+      </c>
+      <c r="AD15" s="2">
+        <f t="shared" si="5"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="AE15" s="4">
+        <f>SUM('Week 1 Total'!AE15,'Week 2 Total'!AE15,'Week 3 Total'!AE15,'Week 4 Total'!AE15)</f>
+        <v>5</v>
+      </c>
+      <c r="AF15" s="4">
+        <f>SUM('Week 1 Total'!AF15,'Week 2 Total'!AF15,'Week 3 Total'!AF15,'Week 4 Total'!AF15)</f>
+        <v>4</v>
+      </c>
+      <c r="AG15" s="4">
+        <f>SUM('Week 1 Total'!AG15,'Week 2 Total'!AG15,'Week 3 Total'!AG15,'Week 4 Total'!AG15)</f>
+        <v>1</v>
+      </c>
+      <c r="AH15" s="2">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="AI15" s="4">
+        <f>SUM('Week 1 Total'!AI15,'Week 2 Total'!AI15,'Week 3 Total'!AI15,'Week 4 Total'!AI15)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="4">
+        <f>SUM('Week 1 Total'!AJ15,'Week 2 Total'!AJ15,'Week 3 Total'!AJ15,'Week 4 Total'!AJ15)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="4">
+        <f>SUM('Week 1 Total'!C16,'Week 2 Total'!C16,'Week 3 Total'!C16,'Week 4 Total'!C16)</f>
+        <v>15</v>
+      </c>
+      <c r="D16" s="4">
+        <f>SUM('Week 1 Total'!D16,'Week 2 Total'!D16,'Week 3 Total'!D16,'Week 4 Total'!D16)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <f>SUM('Week 1 Total'!E16,'Week 2 Total'!E16,'Week 3 Total'!E16,'Week 4 Total'!E16)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <f>SUM('Week 1 Total'!F16,'Week 2 Total'!F16,'Week 3 Total'!F16,'Week 4 Total'!F16)</f>
+        <v>6</v>
+      </c>
+      <c r="G16" s="4">
+        <f>SUM('Week 1 Total'!G16,'Week 2 Total'!G16,'Week 3 Total'!G16,'Week 4 Total'!G16)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <f>SUM('Week 1 Total'!H16,'Week 2 Total'!H16,'Week 3 Total'!H16,'Week 4 Total'!H16)</f>
+        <v>3</v>
+      </c>
+      <c r="I16" s="4">
+        <f>SUM('Week 1 Total'!I16,'Week 2 Total'!I16,'Week 3 Total'!I16,'Week 4 Total'!I16)</f>
+        <v>1</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K16" s="4">
+        <f>SUM('Week 1 Total'!K16,'Week 2 Total'!K16,'Week 3 Total'!K16,'Week 4 Total'!K16)</f>
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
+        <f>SUM('Week 1 Total'!L16,'Week 2 Total'!L16,'Week 3 Total'!L16,'Week 4 Total'!L16)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <f>SUM('Week 1 Total'!M16,'Week 2 Total'!M16,'Week 3 Total'!M16,'Week 4 Total'!M16)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <f>SUM('Week 1 Total'!N16,'Week 2 Total'!N16,'Week 3 Total'!N16,'Week 4 Total'!N16)</f>
+        <v>6</v>
+      </c>
+      <c r="O16" s="4">
+        <f>SUM('Week 1 Total'!O16,'Week 2 Total'!O16,'Week 3 Total'!O16,'Week 4 Total'!O16)</f>
+        <v>2</v>
+      </c>
+      <c r="P16" s="4">
+        <f>SUM('Week 1 Total'!P16,'Week 2 Total'!P16,'Week 3 Total'!P16,'Week 4 Total'!P16)</f>
+        <v>4</v>
+      </c>
+      <c r="Q16" s="4">
+        <f>SUM('Week 1 Total'!Q16,'Week 2 Total'!Q16,'Week 3 Total'!Q16,'Week 4 Total'!Q16)</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="4">
+        <f>SUM('Week 1 Total'!R16,'Week 2 Total'!R16,'Week 3 Total'!R16,'Week 4 Total'!R16)</f>
+        <v>4</v>
+      </c>
+      <c r="S16" s="4">
+        <f>SUM('Week 1 Total'!S16,'Week 2 Total'!S16,'Week 3 Total'!S16,'Week 4 Total'!S16)</f>
+        <v>2</v>
+      </c>
+      <c r="T16" s="4">
+        <f>SUM('Week 1 Total'!T16,'Week 2 Total'!T16,'Week 3 Total'!T16,'Week 4 Total'!T16)</f>
+        <v>2</v>
+      </c>
+      <c r="U16" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4">
+        <f>SUM('Week 1 Total'!W16,'Week 2 Total'!W16,'Week 3 Total'!W16,'Week 4 Total'!W16)</f>
+        <v>3</v>
+      </c>
+      <c r="X16" s="4">
+        <f>SUM('Week 1 Total'!X16,'Week 2 Total'!X16,'Week 3 Total'!X16,'Week 4 Total'!X16)</f>
+        <v>1</v>
+      </c>
+      <c r="Y16" s="4">
+        <f>SUM('Week 1 Total'!Y16,'Week 2 Total'!Y16,'Week 3 Total'!Y16,'Week 4 Total'!Y16)</f>
+        <v>2</v>
+      </c>
+      <c r="Z16" s="2">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA16" s="4">
+        <f>SUM('Week 1 Total'!AA16,'Week 2 Total'!AA16,'Week 3 Total'!AA16,'Week 4 Total'!AA16)</f>
+        <v>1</v>
+      </c>
+      <c r="AB16" s="4">
+        <f>SUM('Week 1 Total'!AB16,'Week 2 Total'!AB16,'Week 3 Total'!AB16,'Week 4 Total'!AB16)</f>
+        <v>1</v>
+      </c>
+      <c r="AC16" s="4">
+        <f>SUM('Week 1 Total'!AC16,'Week 2 Total'!AC16,'Week 3 Total'!AC16,'Week 4 Total'!AC16)</f>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AE16" s="4">
+        <f>SUM('Week 1 Total'!AE16,'Week 2 Total'!AE16,'Week 3 Total'!AE16,'Week 4 Total'!AE16)</f>
+        <v>2</v>
+      </c>
+      <c r="AF16" s="4">
+        <f>SUM('Week 1 Total'!AF16,'Week 2 Total'!AF16,'Week 3 Total'!AF16,'Week 4 Total'!AF16)</f>
+        <v>1</v>
+      </c>
+      <c r="AG16" s="4">
+        <f>SUM('Week 1 Total'!AG16,'Week 2 Total'!AG16,'Week 3 Total'!AG16,'Week 4 Total'!AG16)</f>
+        <v>1</v>
+      </c>
+      <c r="AH16" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="AI16" s="4">
+        <f>SUM('Week 1 Total'!AI16,'Week 2 Total'!AI16,'Week 3 Total'!AI16,'Week 4 Total'!AI16)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="4">
+        <f>SUM('Week 1 Total'!AJ16,'Week 2 Total'!AJ16,'Week 3 Total'!AJ16,'Week 4 Total'!AJ16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="4">
+        <f>SUM('Week 1 Total'!C17,'Week 2 Total'!C17,'Week 3 Total'!C17,'Week 4 Total'!C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <f>SUM('Week 1 Total'!D17,'Week 2 Total'!D17,'Week 3 Total'!D17,'Week 4 Total'!D17)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <f>SUM('Week 1 Total'!E17,'Week 2 Total'!E17,'Week 3 Total'!E17,'Week 4 Total'!E17)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <f>SUM('Week 1 Total'!F17,'Week 2 Total'!F17,'Week 3 Total'!F17,'Week 4 Total'!F17)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <f>SUM('Week 1 Total'!G17,'Week 2 Total'!G17,'Week 3 Total'!G17,'Week 4 Total'!G17)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <f>SUM('Week 1 Total'!H17,'Week 2 Total'!H17,'Week 3 Total'!H17,'Week 4 Total'!H17)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <f>SUM('Week 1 Total'!I17,'Week 2 Total'!I17,'Week 3 Total'!I17,'Week 4 Total'!I17)</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="K17" s="4">
+        <f>SUM('Week 1 Total'!K17,'Week 2 Total'!K17,'Week 3 Total'!K17,'Week 4 Total'!K17)</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <f>SUM('Week 1 Total'!L17,'Week 2 Total'!L17,'Week 3 Total'!L17,'Week 4 Total'!L17)</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
+        <f>SUM('Week 1 Total'!M17,'Week 2 Total'!M17,'Week 3 Total'!M17,'Week 4 Total'!M17)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <f>SUM('Week 1 Total'!N17,'Week 2 Total'!N17,'Week 3 Total'!N17,'Week 4 Total'!N17)</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <f>SUM('Week 1 Total'!O17,'Week 2 Total'!O17,'Week 3 Total'!O17,'Week 4 Total'!O17)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="4">
+        <f>SUM('Week 1 Total'!P17,'Week 2 Total'!P17,'Week 3 Total'!P17,'Week 4 Total'!P17)</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4">
+        <f>SUM('Week 1 Total'!Q17,'Week 2 Total'!Q17,'Week 3 Total'!Q17,'Week 4 Total'!Q17)</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="4">
+        <f>SUM('Week 1 Total'!R17,'Week 2 Total'!R17,'Week 3 Total'!R17,'Week 4 Total'!R17)</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="4">
+        <f>SUM('Week 1 Total'!S17,'Week 2 Total'!S17,'Week 3 Total'!S17,'Week 4 Total'!S17)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="4">
+        <f>SUM('Week 1 Total'!T17,'Week 2 Total'!T17,'Week 3 Total'!T17,'Week 4 Total'!T17)</f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4">
+        <f>SUM('Week 1 Total'!W17,'Week 2 Total'!W17,'Week 3 Total'!W17,'Week 4 Total'!W17)</f>
+        <v>0</v>
+      </c>
+      <c r="X17" s="4">
+        <f>SUM('Week 1 Total'!X17,'Week 2 Total'!X17,'Week 3 Total'!X17,'Week 4 Total'!X17)</f>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="4">
+        <f>SUM('Week 1 Total'!Y17,'Week 2 Total'!Y17,'Week 3 Total'!Y17,'Week 4 Total'!Y17)</f>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA17" s="4">
+        <f>SUM('Week 1 Total'!AA17,'Week 2 Total'!AA17,'Week 3 Total'!AA17,'Week 4 Total'!AA17)</f>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="4">
+        <f>SUM('Week 1 Total'!AB17,'Week 2 Total'!AB17,'Week 3 Total'!AB17,'Week 4 Total'!AB17)</f>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="4">
+        <f>SUM('Week 1 Total'!AC17,'Week 2 Total'!AC17,'Week 3 Total'!AC17,'Week 4 Total'!AC17)</f>
+        <v>0</v>
+      </c>
+      <c r="AD17" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="4">
+        <f>SUM('Week 1 Total'!AE17,'Week 2 Total'!AE17,'Week 3 Total'!AE17,'Week 4 Total'!AE17)</f>
+        <v>0</v>
+      </c>
+      <c r="AF17" s="4">
+        <f>SUM('Week 1 Total'!AF17,'Week 2 Total'!AF17,'Week 3 Total'!AF17,'Week 4 Total'!AF17)</f>
+        <v>0</v>
+      </c>
+      <c r="AG17" s="4">
+        <f>SUM('Week 1 Total'!AG17,'Week 2 Total'!AG17,'Week 3 Total'!AG17,'Week 4 Total'!AG17)</f>
+        <v>0</v>
+      </c>
+      <c r="AH17" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AI17" s="4">
+        <f>SUM('Week 1 Total'!AI17,'Week 2 Total'!AI17,'Week 3 Total'!AI17,'Week 4 Total'!AI17)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="4">
+        <f>SUM('Week 1 Total'!AJ17,'Week 2 Total'!AJ17,'Week 3 Total'!AJ17,'Week 4 Total'!AJ17)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>